<commit_message>
Correcion del excel de la f2
</commit_message>
<xml_diff>
--- a/GE3_TestCasesTemplate_v1.0_F2.xlsx
+++ b/GE3_TestCasesTemplate_v1.0_F2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\PycharmProjects\G81.T17.EG3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C3EEB9-6219-43C5-9829-0E9C3EBE0205}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B79D09-9D5D-4D48-BC66-13F9FC92FA28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="246">
   <si>
     <t>&lt;valid hash for these values&gt;</t>
   </si>
@@ -769,6 +769,9 @@
   </si>
   <si>
     <t>Fichero Json incorrecto: el valor del dato1 se repite</t>
+  </si>
+  <si>
+    <t>Fichero Json incorrecto: se repite el valor del dato3</t>
   </si>
 </sst>
 </file>
@@ -1045,18 +1048,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_3" displayName="Table_3" ref="A1:J54" headerRowDxfId="2" dataDxfId="0" totalsRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_3" displayName="Table_3" ref="A1:J54" headerRowDxfId="12" dataDxfId="11" totalsRowDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NODE" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TERMINAL  (T) / NO TERMINAL (NT)" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="TYPE (DUPLICATION / DELETION / MODIFICATION / VALID)" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ID TEST" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="DESCRIPTION" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FILE PATH" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="FILE CONTENT" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EXPECTED RESULT" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="OBSERVATIONS" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NODE" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TERMINAL  (T) / NO TERMINAL (NT)" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="TYPE (DUPLICATION / DELETION / MODIFICATION / VALID)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ID TEST" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="DESCRIPTION" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FILE PATH" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="FILE CONTENT" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EXPECTED RESULT" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="OBSERVATIONS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="GE3 2021 F2-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1361,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2128,7 +2131,7 @@
         <v>104</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>148</v>
+        <v>245</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>150</v>

</xml_diff>